<commit_message>
Some description soil (FAo Classification)
</commit_message>
<xml_diff>
--- a/Inputs_database/Precipitacion y temperatura.xlsx
+++ b/Inputs_database/Precipitacion y temperatura.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Rafael\Mis documentos Rafael\PROYECTO 2014\Muestreo bosques\Datos muestreo Bosques\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/aeefe507ba652255/Doctorate/quercus_informations/Inputs_database/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A533E399-BF23-431C-949F-1D4791C32728}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="89" documentId="13_ncr:1_{A533E399-BF23-431C-949F-1D4791C32728}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{0D6FFE06-7D9C-4101-B99A-B6F8B041B0F0}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1005" yWindow="-120" windowWidth="19605" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="39">
   <si>
     <t>Provincia</t>
   </si>
@@ -75,6 +75,75 @@
   </si>
   <si>
     <t>TM World Clim</t>
+  </si>
+  <si>
+    <t>Tipos de suelos</t>
+  </si>
+  <si>
+    <t>Clima</t>
+  </si>
+  <si>
+    <t>Csa</t>
+  </si>
+  <si>
+    <t>Luvisoles crómicos com Cambisoles cálcicos y Litosoles</t>
+  </si>
+  <si>
+    <t>Cambisoles cálcicos , Regosoles calcáreos y Litosoles com Rendsinas</t>
+  </si>
+  <si>
+    <t>Litosoles, Luvisoles crómicos y Rendsinas com Cambisoles cálcicos</t>
+  </si>
+  <si>
+    <t>Csa/Csb</t>
+  </si>
+  <si>
+    <t>Regosoles eútricos, Litosoles y Cambisoles eútricos com Rankers sobre materiales metamórficos</t>
+  </si>
+  <si>
+    <t>Regosoles eútricos, Litosoles y Cambisoles eútricos com Rankers sobre materiales plutónicos</t>
+  </si>
+  <si>
+    <t>Regosoles calcáreos y Cambisoles cálcicos com Litosolos, Fluvisolos calcáreos y Rendsinas</t>
+  </si>
+  <si>
+    <t>Cambisoles éutricos, Regosoles éutricos y Litosoles com Rankers</t>
+  </si>
+  <si>
+    <t>Luvisoles crómicos com Cambisoles éutricos y Litosoles</t>
+  </si>
+  <si>
+    <t>Csb</t>
+  </si>
+  <si>
+    <t>Id lrnasa 68</t>
+  </si>
+  <si>
+    <t>(LPq) Leptosol lítico + (CMu) Cambisol húmico/(LPu) Leptosol úmbrico + (RGd) Regosol dístrico</t>
+  </si>
+  <si>
+    <t>Id lrnasa 19</t>
+  </si>
+  <si>
+    <t>CMd Cambisol dístrico y LPq Leptosol lítico, textura média(LPu)/(CMu) Cambisol húmico</t>
+  </si>
+  <si>
+    <t>(CMd) Cambisol dístrico + (CMu) Cambisol húmico/(CMx) Cambisol crómico + (ACh) Acrisol háplico</t>
+  </si>
+  <si>
+    <t>(ACh) Acrisol háplico + (ACu) Acrisol húmico/(CMd) Cambisol dístrico + (ACg) Acrisol gleíco</t>
+  </si>
+  <si>
+    <t>(ACg) Acrisol gleíco + (ACu) Acrisol húmico/(CMg) Cambisol gleíco + (CMu) Cambisol húmico</t>
+  </si>
+  <si>
+    <t>(CMg) Cambisol gleíco + (CMu) Cambisol húmico/(LPq) Leptosol lítico + (CMd) Cambisol dístrico</t>
+  </si>
+  <si>
+    <t>(CMe) Cambisol eútrico + (CMx) Cambisol crómico/(FLc) Fluvisol calcárico + (RGe) Regosol eútrico</t>
+  </si>
+  <si>
+    <t>(CMu) Cambisol húmico + (CMg) Cambisol gleíco/(LPq) Leptosol lítico + (CMd) Cambisol dístrico</t>
   </si>
 </sst>
 </file>
@@ -223,7 +292,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="es-ES"/>
+  <c:lang val="pt-BR"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -241,8 +310,8 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="9.166666666666666E-2"/>
-          <c:y val="4.8611111111111112E-2"/>
+          <c:x val="0.10555555555555556"/>
+          <c:y val="7.1759259259259259E-2"/>
           <c:w val="0.8520833333333333"/>
           <c:h val="0.84027777777777779"/>
         </c:manualLayout>
@@ -317,7 +386,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="es-ES"/>
+                  <a:endParaRPr lang="pt-BR"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -590,7 +659,7 @@
                 <a:cs typeface="Calibri"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-ES"/>
+            <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="63895808"/>
@@ -652,7 +721,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-ES"/>
+            <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="63894272"/>
@@ -692,7 +761,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-ES"/>
+      <a:endParaRPr lang="pt-BR"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -706,7 +775,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="es-ES"/>
+  <c:lang val="pt-BR"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -780,7 +849,7 @@
                       <a:cs typeface="Arial"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="es-ES"/>
+                  <a:endParaRPr lang="pt-BR"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -1073,7 +1142,7 @@
                 <a:cs typeface="Arial"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-ES"/>
+            <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="63527552"/>
@@ -1152,7 +1221,7 @@
                 <a:cs typeface="Arial"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-ES"/>
+            <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="63525632"/>
@@ -1198,7 +1267,7 @@
           <a:cs typeface="Arial"/>
         </a:defRPr>
       </a:pPr>
-      <a:endParaRPr lang="es-ES"/>
+      <a:endParaRPr lang="pt-BR"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1212,7 +1281,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="es-ES"/>
+  <c:lang val="pt-BR"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1296,7 +1365,7 @@
                       <a:cs typeface="Arial"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="es-ES"/>
+                  <a:endParaRPr lang="pt-BR"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -1590,7 +1659,7 @@
                 <a:cs typeface="Arial"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-ES"/>
+            <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="66609920"/>
@@ -1671,7 +1740,7 @@
                 <a:cs typeface="Arial"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-ES"/>
+            <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="66587264"/>
@@ -1718,7 +1787,7 @@
           <a:cs typeface="Arial"/>
         </a:defRPr>
       </a:pPr>
-      <a:endParaRPr lang="es-ES"/>
+      <a:endParaRPr lang="pt-BR"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1733,16 +1802,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>657225</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>657225</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1771,13 +1840,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>247650</xdr:colOff>
       <xdr:row>23</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
+      <xdr:col>21</xdr:col>
       <xdr:colOff>104775</xdr:colOff>
       <xdr:row>39</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
@@ -1810,15 +1879,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>533400</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:colOff>647700</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1849,7 +1918,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1891,7 +1960,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -1943,7 +2012,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -2145,15 +2214,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M31"/>
+  <dimension ref="A1:O31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K2" activeCellId="1" sqref="B2:B31 K2:K31"/>
+      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="15" max="15" width="88.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -2181,8 +2254,14 @@
       <c r="K1" s="6" t="s">
         <v>15</v>
       </c>
+      <c r="M1" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="O1" s="6" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -2211,8 +2290,17 @@
       <c r="K2">
         <v>14.9</v>
       </c>
+      <c r="M2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N2">
+        <v>52</v>
+      </c>
+      <c r="O2" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -2241,8 +2329,17 @@
       <c r="K3">
         <v>16</v>
       </c>
+      <c r="M3" t="s">
+        <v>22</v>
+      </c>
+      <c r="N3">
+        <v>44</v>
+      </c>
+      <c r="O3" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -2271,8 +2368,17 @@
       <c r="K4">
         <v>15.3</v>
       </c>
+      <c r="M4" t="s">
+        <v>18</v>
+      </c>
+      <c r="N4">
+        <v>19</v>
+      </c>
+      <c r="O4" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -2301,8 +2407,17 @@
       <c r="K5">
         <v>15.9</v>
       </c>
+      <c r="M5" t="s">
+        <v>22</v>
+      </c>
+      <c r="N5">
+        <v>44</v>
+      </c>
+      <c r="O5" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -2331,8 +2446,17 @@
       <c r="K6">
         <v>16</v>
       </c>
+      <c r="M6" t="s">
+        <v>22</v>
+      </c>
+      <c r="N6">
+        <v>44</v>
+      </c>
+      <c r="O6" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -2361,8 +2485,17 @@
       <c r="K7">
         <v>16.3</v>
       </c>
+      <c r="M7" t="s">
+        <v>18</v>
+      </c>
+      <c r="N7">
+        <v>5</v>
+      </c>
+      <c r="O7" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -2391,8 +2524,17 @@
       <c r="K8">
         <v>15.9</v>
       </c>
+      <c r="M8" t="s">
+        <v>18</v>
+      </c>
+      <c r="N8">
+        <v>6</v>
+      </c>
+      <c r="O8" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -2421,8 +2563,17 @@
       <c r="K9">
         <v>16.600000000000001</v>
       </c>
+      <c r="M9" t="s">
+        <v>18</v>
+      </c>
+      <c r="N9">
+        <v>13</v>
+      </c>
+      <c r="O9" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -2451,8 +2602,17 @@
       <c r="K10">
         <v>16.7</v>
       </c>
+      <c r="M10" t="s">
+        <v>18</v>
+      </c>
+      <c r="N10">
+        <v>5</v>
+      </c>
+      <c r="O10" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -2481,8 +2641,17 @@
       <c r="K11">
         <v>17.3</v>
       </c>
+      <c r="M11" t="s">
+        <v>18</v>
+      </c>
+      <c r="N11">
+        <v>5</v>
+      </c>
+      <c r="O11" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -2514,8 +2683,12 @@
       <c r="L12" s="15">
         <v>272907</v>
       </c>
+      <c r="M12" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="N12" s="16"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -2547,8 +2720,12 @@
       <c r="L13" s="15">
         <v>272907</v>
       </c>
+      <c r="M13" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="N13" s="16"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>10</v>
       </c>
@@ -2578,8 +2755,12 @@
         <v>12.1</v>
       </c>
       <c r="L14" s="16"/>
+      <c r="M14" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="N14" s="16"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>10</v>
       </c>
@@ -2609,8 +2790,12 @@
         <v>12.9</v>
       </c>
       <c r="L15" s="16"/>
+      <c r="M15" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="N15" s="16"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>10</v>
       </c>
@@ -2640,8 +2825,12 @@
         <v>13.1</v>
       </c>
       <c r="L16" s="16"/>
+      <c r="M16" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="N16" s="16"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>11</v>
       </c>
@@ -2673,8 +2862,17 @@
       <c r="L17" s="17">
         <v>410144</v>
       </c>
+      <c r="M17" t="s">
+        <v>18</v>
+      </c>
+      <c r="N17" s="17">
+        <v>31</v>
+      </c>
+      <c r="O17" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>11</v>
       </c>
@@ -2704,8 +2902,17 @@
         <v>15.3</v>
       </c>
       <c r="L18" s="16"/>
+      <c r="M18" t="s">
+        <v>18</v>
+      </c>
+      <c r="N18" s="16">
+        <v>31</v>
+      </c>
+      <c r="O18" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>11</v>
       </c>
@@ -2735,8 +2942,17 @@
         <v>15.5</v>
       </c>
       <c r="L19" s="16"/>
+      <c r="M19" t="s">
+        <v>18</v>
+      </c>
+      <c r="N19" s="16">
+        <v>56</v>
+      </c>
+      <c r="O19" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>11</v>
       </c>
@@ -2766,8 +2982,17 @@
         <v>15</v>
       </c>
       <c r="L20" s="16"/>
+      <c r="M20" t="s">
+        <v>18</v>
+      </c>
+      <c r="N20" s="16">
+        <v>31</v>
+      </c>
+      <c r="O20" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>11</v>
       </c>
@@ -2797,8 +3022,17 @@
         <v>14.9</v>
       </c>
       <c r="L21" s="16"/>
+      <c r="M21" t="s">
+        <v>18</v>
+      </c>
+      <c r="N21" s="16">
+        <v>31</v>
+      </c>
+      <c r="O21" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>12</v>
       </c>
@@ -2830,9 +3064,17 @@
       <c r="L22" s="17">
         <v>4501102</v>
       </c>
-      <c r="M22" s="13"/>
+      <c r="M22" t="s">
+        <v>18</v>
+      </c>
+      <c r="N22" s="17">
+        <v>94</v>
+      </c>
+      <c r="O22" t="s">
+        <v>38</v>
+      </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>12</v>
       </c>
@@ -2862,8 +3104,12 @@
         <v>14.9</v>
       </c>
       <c r="L23" s="16"/>
+      <c r="M23" t="s">
+        <v>18</v>
+      </c>
+      <c r="N23" s="16"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>12</v>
       </c>
@@ -2893,8 +3139,17 @@
         <v>15.4</v>
       </c>
       <c r="L24" s="16"/>
+      <c r="M24" t="s">
+        <v>18</v>
+      </c>
+      <c r="N24" s="16">
+        <v>59</v>
+      </c>
+      <c r="O24" t="s">
+        <v>37</v>
+      </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>12</v>
       </c>
@@ -2924,8 +3179,17 @@
         <v>14.4</v>
       </c>
       <c r="L25" s="16"/>
+      <c r="M25" t="s">
+        <v>18</v>
+      </c>
+      <c r="N25" s="16">
+        <v>109</v>
+      </c>
+      <c r="O25" t="s">
+        <v>36</v>
+      </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>12</v>
       </c>
@@ -2957,8 +3221,12 @@
       <c r="L26" s="15">
         <v>451336</v>
       </c>
+      <c r="M26" t="s">
+        <v>18</v>
+      </c>
+      <c r="N26" s="15"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>13</v>
       </c>
@@ -2988,8 +3256,17 @@
         <v>10.9</v>
       </c>
       <c r="L27" s="16"/>
+      <c r="M27" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="N27" t="s">
+        <v>31</v>
+      </c>
+      <c r="O27" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>13</v>
       </c>
@@ -3019,8 +3296,17 @@
         <v>10.9</v>
       </c>
       <c r="L28" s="16"/>
+      <c r="M28" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="N28" s="16">
+        <v>75</v>
+      </c>
+      <c r="O28" t="s">
+        <v>33</v>
+      </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>13</v>
       </c>
@@ -3050,8 +3336,17 @@
         <v>11.4</v>
       </c>
       <c r="L29" s="16"/>
+      <c r="M29" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="N29">
+        <v>168</v>
+      </c>
+      <c r="O29" t="s">
+        <v>34</v>
+      </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>13</v>
       </c>
@@ -3083,8 +3378,17 @@
       <c r="L30" s="18">
         <v>490524</v>
       </c>
+      <c r="M30" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="N30" s="18">
+        <v>175</v>
+      </c>
+      <c r="O30" t="s">
+        <v>35</v>
+      </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>13</v>
       </c>
@@ -3114,10 +3418,19 @@
         <v>12</v>
       </c>
       <c r="L31" s="16"/>
+      <c r="M31" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="N31" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="O31" t="s">
+        <v>32</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="L12:L13 L26">
+  <conditionalFormatting sqref="L26 L12:L13 N26">
     <cfRule type="expression" dxfId="0" priority="1" stopIfTrue="1">
       <formula>AND(COUNTIF($A$2:$A$6916, L12)&gt;1,NOT(ISBLANK(L12)))</formula>
     </cfRule>

</xml_diff>